<commit_message>
Initial version of tracker schematic
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github.com\zachdeibert\radio-tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C97CC2B-5536-4072-9AAA-70B3B206F9B7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC6A236-DA28-4374-B924-33610A286A6B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B5C8F384-52A8-4954-BEC8-251D2703848F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="125">
   <si>
     <t>Part</t>
   </si>
@@ -336,9 +336,6 @@
     <t>2-1825910-7</t>
   </si>
   <si>
-    <t>https://www.digikey.com/product-detail/en/te-connectivity-alcoswitch-switches/2-1825910-7/450-1642-ND/1632528</t>
-  </si>
-  <si>
     <t>https://www.te.com/commerce/DocumentDelivery/DDEController?Action=srchrtrv&amp;DocNm=1825910&amp;DocType=Customer+Drawing&amp;DocLang=English</t>
   </si>
   <si>
@@ -352,6 +349,63 @@
   </si>
   <si>
     <t>https://www.diodes.com/assets/Datasheets/DMG2302UK.pdf</t>
+  </si>
+  <si>
+    <t>EEPROM</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/stmicroelectronics/M24128-BRMN6TP/497-8619-1-ND/2038663</t>
+  </si>
+  <si>
+    <t>https://www.st.com/content/ccc/resource/technical/document/datasheet/59/05/c9/5b/7b/41/48/b6/CD00259167.pdf/files/CD00259167.pdf/jcr:content/translations/en.CD00259167.pdf</t>
+  </si>
+  <si>
+    <t>~ M24128-BRMN6TP</t>
+  </si>
+  <si>
+    <t>http://ww1.microchip.com/downloads/en/DeviceDoc/40001906C.pdf</t>
+  </si>
+  <si>
+    <t>https://www.waveshare.com/datasheet/LCD_en_PDF/ST7920.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/te-connectivity-alcoswitch-switches/3-1825910-1/450-1643-ND/1632529</t>
+  </si>
+  <si>
+    <t>Power Switch</t>
+  </si>
+  <si>
+    <t>OS102011MA1QN1</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/c-k/OS102011MA1QN1/CKN9559-ND/1981430</t>
+  </si>
+  <si>
+    <t>https://www.ckswitches.com/media/1428/os.pdf</t>
+  </si>
+  <si>
+    <t>Voltage Reference</t>
+  </si>
+  <si>
+    <t>MCP1501T-30E/CHY</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/microchip-technology/MCP1501T-30E-CHY/MCP1501T-30E-CHYCT-ND/5844633</t>
+  </si>
+  <si>
+    <t>http://ww1.microchip.com/downloads/en/DeviceDoc/20005474E.pdf</t>
+  </si>
+  <si>
+    <t>Trimmer</t>
+  </si>
+  <si>
+    <t>TC33X-2-103E</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/bourns-inc/TC33X-2-103E/TC33X-103ECT-ND/612911</t>
+  </si>
+  <si>
+    <t>https://www.bourns.com/docs/Product-Datasheets/TC33.pdf</t>
   </si>
 </sst>
 </file>
@@ -415,7 +469,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
@@ -423,6 +477,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -739,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF14E9F-6EA3-4C47-9EC5-A7065BD25A1E}">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,10 +814,11 @@
     <col min="8" max="8" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="120.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="138" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="169.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="64" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -791,11 +849,12 @@
       <c r="J1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="7"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -827,7 +886,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -859,7 +918,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -891,7 +950,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -923,7 +982,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -955,7 +1014,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -987,7 +1046,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1016,7 +1075,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1051,7 +1110,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1086,7 +1145,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1118,7 +1177,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -1150,7 +1209,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -1182,7 +1241,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -1214,7 +1273,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1245,8 +1304,11 @@
       <c r="K15" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>64</v>
       </c>
@@ -1278,7 +1340,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -1310,7 +1372,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -1342,7 +1404,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -1377,12 +1439,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20" t="s">
         <v>103</v>
-      </c>
-      <c r="B20" t="s">
-        <v>104</v>
       </c>
       <c r="C20" s="3">
         <v>0.33</v>
@@ -1406,13 +1468,13 @@
         <v>0.33</v>
       </c>
       <c r="J20" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K20" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="K20" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>80</v>
       </c>
@@ -1444,7 +1506,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>84</v>
       </c>
@@ -1476,7 +1538,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>88</v>
       </c>
@@ -1508,7 +1570,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>92</v>
       </c>
@@ -1533,8 +1595,11 @@
       <c r="K24" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>95</v>
       </c>
@@ -1548,15 +1613,15 @@
         <v>1</v>
       </c>
       <c r="G25" s="3">
-        <f t="shared" ref="G25:G26" si="5">$C25*D25</f>
+        <f t="shared" ref="G25:G30" si="5">$C25*D25</f>
         <v>1.7</v>
       </c>
       <c r="H25" s="3">
-        <f t="shared" ref="H25:H26" si="6">$C25*E25</f>
+        <f t="shared" ref="H25:H30" si="6">$C25*E25</f>
         <v>0</v>
       </c>
       <c r="I25" s="3">
-        <f t="shared" ref="I25:I26" si="7">$C25*F25</f>
+        <f t="shared" ref="I25:I30" si="7">$C25*F25</f>
         <v>0</v>
       </c>
       <c r="J25" s="2" t="s">
@@ -1566,7 +1631,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>99</v>
       </c>
@@ -1574,14 +1639,14 @@
         <v>100</v>
       </c>
       <c r="C26" s="3">
-        <v>0.114</v>
+        <v>0.18</v>
       </c>
       <c r="D26" s="6">
         <v>12</v>
       </c>
       <c r="G26" s="3">
         <f t="shared" si="5"/>
-        <v>1.3680000000000001</v>
+        <v>2.16</v>
       </c>
       <c r="H26" s="3">
         <f t="shared" si="6"/>
@@ -1592,13 +1657,144 @@
         <v>0</v>
       </c>
       <c r="J26" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="K26" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="K26" s="2" t="s">
-        <v>102</v>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.26</v>
+      </c>
+      <c r="D27" s="6">
+        <v>1</v>
+      </c>
+      <c r="G27" s="3">
+        <f t="shared" si="5"/>
+        <v>0.26</v>
+      </c>
+      <c r="H27" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>113</v>
+      </c>
+      <c r="B28" t="s">
+        <v>114</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0.48</v>
+      </c>
+      <c r="D28" s="6">
+        <v>1</v>
+      </c>
+      <c r="G28" s="3">
+        <f t="shared" si="5"/>
+        <v>0.48</v>
+      </c>
+      <c r="H28" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>117</v>
+      </c>
+      <c r="B29" t="s">
+        <v>118</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0.76</v>
+      </c>
+      <c r="D29" s="6">
+        <v>1</v>
+      </c>
+      <c r="G29" s="3">
+        <f t="shared" si="5"/>
+        <v>0.76</v>
+      </c>
+      <c r="H29" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>121</v>
+      </c>
+      <c r="B30" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D30" s="6">
+        <v>1</v>
+      </c>
+      <c r="G30" s="3">
+        <f t="shared" si="5"/>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H30" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I30" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="K1:L1"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="K5" r:id="rId1" xr:uid="{B1C6F00B-EA48-4262-90C1-FABF9D9B7E15}"/>
     <hyperlink ref="K4" r:id="rId2" xr:uid="{B2BF729A-B344-4D4E-918B-E150F708DAF6}"/>
@@ -1649,8 +1845,18 @@
     <hyperlink ref="K26" r:id="rId47" xr:uid="{A220C75B-2B93-4FFA-83FF-80385D4BAC5E}"/>
     <hyperlink ref="J20" r:id="rId48" xr:uid="{A07C5993-29BD-4CE4-8ACD-DDFE88D68FB2}"/>
     <hyperlink ref="K20" r:id="rId49" xr:uid="{D0A9BC38-F839-4D2F-93B9-A62B36C3CEBF}"/>
+    <hyperlink ref="J27" r:id="rId50" xr:uid="{F9ADDC0D-81CF-4E42-B964-63D4FD61BA13}"/>
+    <hyperlink ref="K27" r:id="rId51" xr:uid="{4F87CAEC-7381-4AAC-92D2-751506D3A161}"/>
+    <hyperlink ref="L15" r:id="rId52" xr:uid="{DECFA331-29DD-4FE7-8BDB-CDE3B2E95E8E}"/>
+    <hyperlink ref="L24" r:id="rId53" xr:uid="{396BB15D-A498-4E98-A64A-2FE1D5019461}"/>
+    <hyperlink ref="J28" r:id="rId54" xr:uid="{FB34B9B4-55E1-47A1-8E21-A821A00D1EC0}"/>
+    <hyperlink ref="K28" r:id="rId55" xr:uid="{C1060359-9B35-48F1-A2D8-AA3BD374A571}"/>
+    <hyperlink ref="J29" r:id="rId56" xr:uid="{BFE70BF4-2F9A-4802-8E95-A3A3490948A8}"/>
+    <hyperlink ref="K29" r:id="rId57" xr:uid="{CE60DCE8-B339-40F0-B2EF-BD73D4938106}"/>
+    <hyperlink ref="J30" r:id="rId58" xr:uid="{3585C032-D124-4147-B5B7-3F2EF6C6A5DE}"/>
+    <hyperlink ref="K30" r:id="rId59" xr:uid="{F22462B9-9A26-48B6-A0DD-B57066B22C40}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId50"/>
+  <pageSetup orientation="portrait" r:id="rId60"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
A few schematic updates
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github.com\zachdeibert\radio-tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B79F7B-E71C-4E1F-907A-FFDFA3542F40}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DEA505E-418E-45EA-8940-DADB69D879C5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B5C8F384-52A8-4954-BEC8-251D2703848F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="146">
   <si>
     <t>Part</t>
   </si>
@@ -138,15 +138,6 @@
     <t>https://assets.nexperia.com/documents/data-sheet/MMBT3904.pdf</t>
   </si>
   <si>
-    <t>https://www.soberton.com/wp-content/uploads/2019/02/WT-1205-16-Feb-2019.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/soberton-inc/WT-1205/433-1028-ND/479674</t>
-  </si>
-  <si>
-    <t>WT-1205</t>
-  </si>
-  <si>
     <t>ABLS</t>
   </si>
   <si>
@@ -457,6 +448,27 @@
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/643075-4/A19232-ND/258868</t>
+  </si>
+  <si>
+    <t>AT-1224-TWT-5V-2-R</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/pui-audio-inc/AT-1224-TWT-5V-2-R/668-1470-ND/5011404</t>
+  </si>
+  <si>
+    <t>http://www.puiaudio.com/pdf/AT-1224-TWT-5V-2-R.pdf</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 	47L16-I/SN</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/microchip-technology/47L16-I-SN/47L16-I-SN-ND/6098090</t>
+  </si>
+  <si>
+    <t>http://ww1.microchip.com/downloads/en/DeviceDoc/47L04_47C04_47L16_47C16_DS20005371D.pdf</t>
   </si>
 </sst>
 </file>
@@ -847,10 +859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF14E9F-6EA3-4C47-9EC5-A7065BD25A1E}">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,25 +892,25 @@
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="K1" s="7" t="s">
         <v>2</v>
@@ -1038,17 +1050,20 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C6" s="3">
         <v>0.43</v>
       </c>
+      <c r="D6" s="6">
+        <v>1</v>
+      </c>
       <c r="E6" s="6">
         <v>1</v>
       </c>
       <c r="G6" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.43</v>
       </c>
       <c r="H6" s="3">
         <f t="shared" si="0"/>
@@ -1166,10 +1181,10 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>139</v>
       </c>
       <c r="C10" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.61</v>
       </c>
       <c r="D10" s="6">
         <v>1</v>
@@ -1179,7 +1194,7 @@
       </c>
       <c r="G10" s="3">
         <f t="shared" si="1"/>
-        <v>0.57999999999999996</v>
+        <v>0.61</v>
       </c>
       <c r="H10" s="3">
         <f t="shared" si="0"/>
@@ -1187,13 +1202,13 @@
       </c>
       <c r="I10" s="3">
         <f t="shared" si="0"/>
-        <v>0.57999999999999996</v>
+        <v>0.61</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>35</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1201,7 +1216,7 @@
         <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C11" s="3">
         <v>0.22</v>
@@ -1222,18 +1237,18 @@
         <v>0.22</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C12" s="3">
         <v>4.95</v>
@@ -1254,18 +1269,18 @@
         <v>0</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C13" s="3">
         <v>1.98</v>
@@ -1286,18 +1301,18 @@
         <v>0</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C14" s="3">
         <v>0</v>
@@ -1318,10 +1333,10 @@
         <v>0</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1329,7 +1344,7 @@
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C15" s="3">
         <v>1.34</v>
@@ -1350,21 +1365,21 @@
         <v>0</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C16" s="3">
         <v>2.39</v>
@@ -1385,18 +1400,18 @@
         <v>0</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C17" s="3">
         <v>1.19</v>
@@ -1417,18 +1432,18 @@
         <v>0</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C18" s="3">
         <v>1.08</v>
@@ -1449,53 +1464,50 @@
         <v>0</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C19" s="3">
         <v>0.11</v>
       </c>
-      <c r="D19" s="6">
-        <v>1</v>
-      </c>
       <c r="E19" s="6">
         <v>1</v>
       </c>
       <c r="G19" s="3">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="3">
+        <f t="shared" si="0"/>
         <v>0.11</v>
       </c>
-      <c r="H19" s="3">
-        <f t="shared" si="0"/>
-        <v>0.11</v>
-      </c>
       <c r="I19" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B20" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C20" s="3">
         <v>0.33</v>
@@ -1519,18 +1531,18 @@
         <v>0.33</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C21" s="3">
         <v>0.35</v>
@@ -1551,18 +1563,18 @@
         <v>0</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C22" s="3">
         <v>0.77</v>
@@ -1583,18 +1595,18 @@
         <v>0</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C23" s="3">
         <v>0.56999999999999995</v>
@@ -1615,18 +1627,18 @@
         <v>0</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B24" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D24" s="6">
         <v>1</v>
@@ -1644,18 +1656,18 @@
         <v>0</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B25" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C25" s="3">
         <v>1.7</v>
@@ -1664,30 +1676,30 @@
         <v>1</v>
       </c>
       <c r="G25" s="3">
-        <f t="shared" ref="G25:G36" si="5">$C25*D25</f>
+        <f t="shared" ref="G25:G37" si="5">$C25*D25</f>
         <v>1.7</v>
       </c>
       <c r="H25" s="3">
-        <f t="shared" ref="H25:H36" si="6">$C25*E25</f>
+        <f t="shared" ref="H25:H37" si="6">$C25*E25</f>
         <v>0</v>
       </c>
       <c r="I25" s="3">
-        <f t="shared" ref="I25:I36" si="7">$C25*F25</f>
+        <f t="shared" ref="I25:I37" si="7">$C25*F25</f>
         <v>0</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B26" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C26" s="3">
         <v>0.18</v>
@@ -1708,18 +1720,18 @@
         <v>0</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" t="s">
         <v>106</v>
-      </c>
-      <c r="B27" t="s">
-        <v>109</v>
       </c>
       <c r="C27" s="3">
         <v>0.26</v>
@@ -1740,18 +1752,18 @@
         <v>0</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B28" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C28" s="3">
         <v>0.48</v>
@@ -1772,18 +1784,18 @@
         <v>0</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B29" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C29" s="3">
         <v>0.76</v>
@@ -1804,18 +1816,18 @@
         <v>0</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B30" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C30" s="3">
         <v>0.28000000000000003</v>
@@ -1836,18 +1848,18 @@
         <v>0</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B31" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C31" s="3">
         <v>3.48</v>
@@ -1868,15 +1880,15 @@
         <v>0</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32" t="s">
         <v>125</v>
-      </c>
-      <c r="B32" t="s">
-        <v>128</v>
       </c>
       <c r="C32" s="3">
         <v>0.124</v>
@@ -1897,15 +1909,15 @@
         <v>0</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B33" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C33" s="3">
         <v>0.78</v>
@@ -1926,15 +1938,15 @@
         <v>0</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B34" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C34" s="3">
         <v>0.14000000000000001</v>
@@ -1955,18 +1967,18 @@
         <v>0</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B35" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C35" s="3">
         <v>0.22</v>
@@ -1987,15 +1999,15 @@
         <v>0</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>134</v>
+      </c>
+      <c r="B36" t="s">
         <v>137</v>
-      </c>
-      <c r="B36" t="s">
-        <v>140</v>
       </c>
       <c r="C36" s="3">
         <v>0.45</v>
@@ -2016,7 +2028,39 @@
         <v>0</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>142</v>
+      </c>
+      <c r="B37" t="s">
+        <v>143</v>
+      </c>
+      <c r="C37" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="D37" s="6">
+        <v>1</v>
+      </c>
+      <c r="G37" s="3">
+        <f t="shared" si="5"/>
+        <v>0.7</v>
+      </c>
+      <c r="H37" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I37" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -2040,58 +2084,60 @@
     <hyperlink ref="K8" r:id="rId14" xr:uid="{8498C100-CDF5-4C06-84D9-7FF915743C55}"/>
     <hyperlink ref="J9" r:id="rId15" xr:uid="{E636B5DC-60F1-4C7A-85D7-F21C14A59AEE}"/>
     <hyperlink ref="K9" r:id="rId16" xr:uid="{821C58E6-92B3-4E82-957D-C74C6923EA8D}"/>
-    <hyperlink ref="K10" r:id="rId17" xr:uid="{2DB8A609-439E-4E56-A558-0EC1E5E5860B}"/>
-    <hyperlink ref="J10" r:id="rId18" xr:uid="{74D8B8FC-5436-4B80-8A75-C5DCBCF7B670}"/>
-    <hyperlink ref="J11" r:id="rId19" xr:uid="{DDDFC995-E04C-42CA-B3D3-777C4BC8A79B}"/>
-    <hyperlink ref="K11" r:id="rId20" xr:uid="{662AE6A5-20FD-445F-A1DA-DC7516A174F3}"/>
-    <hyperlink ref="J12" r:id="rId21" xr:uid="{AB27E188-70B1-44A3-8993-60449F82C023}"/>
-    <hyperlink ref="K12" r:id="rId22" xr:uid="{28A03317-F9CF-43E1-A366-6679378796B9}"/>
-    <hyperlink ref="J13" r:id="rId23" xr:uid="{55AAA167-A2BB-4945-8D01-28CFD81ECE11}"/>
-    <hyperlink ref="K13" r:id="rId24" xr:uid="{077D4FE6-3DBC-4ED6-ABC3-330BF75DDA0E}"/>
-    <hyperlink ref="K14" r:id="rId25" xr:uid="{EB583FFA-96AD-44EB-9088-B4EE0561479C}"/>
-    <hyperlink ref="J14" r:id="rId26" xr:uid="{ACDC732C-7C87-4605-9946-BFB4072A5D15}"/>
-    <hyperlink ref="J15" r:id="rId27" xr:uid="{E3C15645-CFAE-4A73-97B5-F6FD38529D83}"/>
-    <hyperlink ref="K15" r:id="rId28" xr:uid="{CAEC8B72-B4B1-4502-B9E2-883E2B823C57}"/>
-    <hyperlink ref="J16" r:id="rId29" xr:uid="{AE8CF4F1-E710-4357-A6A9-34EC29EB7F29}"/>
-    <hyperlink ref="K16" r:id="rId30" xr:uid="{F22177DA-B5DE-44DE-8257-37582708A997}"/>
-    <hyperlink ref="J17" r:id="rId31" xr:uid="{572584A5-62F3-496C-BB6C-C8354525984D}"/>
-    <hyperlink ref="K17" r:id="rId32" xr:uid="{DA0BEC51-2B2F-4027-A8FB-529C7DE12331}"/>
-    <hyperlink ref="J18" r:id="rId33" xr:uid="{ECF36898-98AC-4601-975C-BD38506FA4F9}"/>
-    <hyperlink ref="K18" r:id="rId34" xr:uid="{A24890BF-4B5E-40CB-B9B4-34A68264736E}"/>
-    <hyperlink ref="J19" r:id="rId35" xr:uid="{8FB6D7D0-23A7-4B02-9810-79304E9FC6DF}"/>
-    <hyperlink ref="K19" r:id="rId36" xr:uid="{F3CA4998-91B4-4D7B-B5CE-EAA22B63412F}"/>
-    <hyperlink ref="J21" r:id="rId37" xr:uid="{7FB55ABB-ED42-4074-86E4-CB5588011F6F}"/>
-    <hyperlink ref="K21" r:id="rId38" xr:uid="{41D3F80A-03BC-477F-82CF-CEBE0D8D65D8}"/>
-    <hyperlink ref="J22" r:id="rId39" xr:uid="{BCD256D2-392F-4BA1-98E8-DAF9918681E6}"/>
-    <hyperlink ref="K22" r:id="rId40" xr:uid="{EED098FB-1018-4864-93D7-093FBEA1E075}"/>
-    <hyperlink ref="J23" r:id="rId41" xr:uid="{866D5E06-28C5-4774-B325-4596BE7F026E}"/>
-    <hyperlink ref="K23" r:id="rId42" xr:uid="{F1429A52-5972-4235-BA2E-8ABDEDFB6995}"/>
-    <hyperlink ref="K24" r:id="rId43" xr:uid="{62B17503-CC61-45E9-91BF-3B440A5FF457}"/>
-    <hyperlink ref="J25" r:id="rId44" xr:uid="{754A96EE-B03B-46E4-A496-9A8227C3ABB1}"/>
-    <hyperlink ref="K25" r:id="rId45" xr:uid="{F9D080CD-142B-443B-ABD0-D6A755886BB2}"/>
-    <hyperlink ref="J26" r:id="rId46" xr:uid="{793B7E3D-F72F-4E0A-93D6-73D47105EEDA}"/>
-    <hyperlink ref="K26" r:id="rId47" xr:uid="{A220C75B-2B93-4FFA-83FF-80385D4BAC5E}"/>
-    <hyperlink ref="J20" r:id="rId48" xr:uid="{A07C5993-29BD-4CE4-8ACD-DDFE88D68FB2}"/>
-    <hyperlink ref="K20" r:id="rId49" xr:uid="{D0A9BC38-F839-4D2F-93B9-A62B36C3CEBF}"/>
-    <hyperlink ref="J27" r:id="rId50" xr:uid="{F9ADDC0D-81CF-4E42-B964-63D4FD61BA13}"/>
-    <hyperlink ref="K27" r:id="rId51" xr:uid="{4F87CAEC-7381-4AAC-92D2-751506D3A161}"/>
-    <hyperlink ref="L15" r:id="rId52" xr:uid="{DECFA331-29DD-4FE7-8BDB-CDE3B2E95E8E}"/>
-    <hyperlink ref="L24" r:id="rId53" xr:uid="{396BB15D-A498-4E98-A64A-2FE1D5019461}"/>
-    <hyperlink ref="J28" r:id="rId54" xr:uid="{FB34B9B4-55E1-47A1-8E21-A821A00D1EC0}"/>
-    <hyperlink ref="K28" r:id="rId55" xr:uid="{C1060359-9B35-48F1-A2D8-AA3BD374A571}"/>
-    <hyperlink ref="J29" r:id="rId56" xr:uid="{BFE70BF4-2F9A-4802-8E95-A3A3490948A8}"/>
-    <hyperlink ref="K29" r:id="rId57" xr:uid="{CE60DCE8-B339-40F0-B2EF-BD73D4938106}"/>
-    <hyperlink ref="J30" r:id="rId58" xr:uid="{3585C032-D124-4147-B5B7-3F2EF6C6A5DE}"/>
-    <hyperlink ref="K30" r:id="rId59" xr:uid="{F22462B9-9A26-48B6-A0DD-B57066B22C40}"/>
-    <hyperlink ref="J31" r:id="rId60" xr:uid="{187F5B61-0870-420A-BB74-16CAAFC01941}"/>
-    <hyperlink ref="J32" r:id="rId61" xr:uid="{680E5967-C777-4D8D-B069-D0D96FFC678B}"/>
-    <hyperlink ref="J33" r:id="rId62" xr:uid="{577FFBCD-009F-478E-8E33-91E761042C29}"/>
-    <hyperlink ref="J34" r:id="rId63" xr:uid="{19F11160-B47A-43B1-9F79-BEA1F1972CA2}"/>
-    <hyperlink ref="K34" r:id="rId64" xr:uid="{752EBF32-C084-4C5C-B069-3517A1A6AE50}"/>
-    <hyperlink ref="J35" r:id="rId65" xr:uid="{9C3C1D94-3708-4CC6-90CF-7C720C888ED2}"/>
-    <hyperlink ref="J36" r:id="rId66" xr:uid="{CDB6AD6E-50EC-4A3E-8C8C-94992C4158F3}"/>
+    <hyperlink ref="J11" r:id="rId17" xr:uid="{DDDFC995-E04C-42CA-B3D3-777C4BC8A79B}"/>
+    <hyperlink ref="K11" r:id="rId18" xr:uid="{662AE6A5-20FD-445F-A1DA-DC7516A174F3}"/>
+    <hyperlink ref="J12" r:id="rId19" xr:uid="{AB27E188-70B1-44A3-8993-60449F82C023}"/>
+    <hyperlink ref="K12" r:id="rId20" xr:uid="{28A03317-F9CF-43E1-A366-6679378796B9}"/>
+    <hyperlink ref="J13" r:id="rId21" xr:uid="{55AAA167-A2BB-4945-8D01-28CFD81ECE11}"/>
+    <hyperlink ref="K13" r:id="rId22" xr:uid="{077D4FE6-3DBC-4ED6-ABC3-330BF75DDA0E}"/>
+    <hyperlink ref="K14" r:id="rId23" xr:uid="{EB583FFA-96AD-44EB-9088-B4EE0561479C}"/>
+    <hyperlink ref="J14" r:id="rId24" xr:uid="{ACDC732C-7C87-4605-9946-BFB4072A5D15}"/>
+    <hyperlink ref="J15" r:id="rId25" xr:uid="{E3C15645-CFAE-4A73-97B5-F6FD38529D83}"/>
+    <hyperlink ref="K15" r:id="rId26" xr:uid="{CAEC8B72-B4B1-4502-B9E2-883E2B823C57}"/>
+    <hyperlink ref="J16" r:id="rId27" xr:uid="{AE8CF4F1-E710-4357-A6A9-34EC29EB7F29}"/>
+    <hyperlink ref="K16" r:id="rId28" xr:uid="{F22177DA-B5DE-44DE-8257-37582708A997}"/>
+    <hyperlink ref="J17" r:id="rId29" xr:uid="{572584A5-62F3-496C-BB6C-C8354525984D}"/>
+    <hyperlink ref="K17" r:id="rId30" xr:uid="{DA0BEC51-2B2F-4027-A8FB-529C7DE12331}"/>
+    <hyperlink ref="J18" r:id="rId31" xr:uid="{ECF36898-98AC-4601-975C-BD38506FA4F9}"/>
+    <hyperlink ref="K18" r:id="rId32" xr:uid="{A24890BF-4B5E-40CB-B9B4-34A68264736E}"/>
+    <hyperlink ref="J19" r:id="rId33" xr:uid="{8FB6D7D0-23A7-4B02-9810-79304E9FC6DF}"/>
+    <hyperlink ref="K19" r:id="rId34" xr:uid="{F3CA4998-91B4-4D7B-B5CE-EAA22B63412F}"/>
+    <hyperlink ref="J21" r:id="rId35" xr:uid="{7FB55ABB-ED42-4074-86E4-CB5588011F6F}"/>
+    <hyperlink ref="K21" r:id="rId36" xr:uid="{41D3F80A-03BC-477F-82CF-CEBE0D8D65D8}"/>
+    <hyperlink ref="J22" r:id="rId37" xr:uid="{BCD256D2-392F-4BA1-98E8-DAF9918681E6}"/>
+    <hyperlink ref="K22" r:id="rId38" xr:uid="{EED098FB-1018-4864-93D7-093FBEA1E075}"/>
+    <hyperlink ref="J23" r:id="rId39" xr:uid="{866D5E06-28C5-4774-B325-4596BE7F026E}"/>
+    <hyperlink ref="K23" r:id="rId40" xr:uid="{F1429A52-5972-4235-BA2E-8ABDEDFB6995}"/>
+    <hyperlink ref="K24" r:id="rId41" xr:uid="{62B17503-CC61-45E9-91BF-3B440A5FF457}"/>
+    <hyperlink ref="J25" r:id="rId42" xr:uid="{754A96EE-B03B-46E4-A496-9A8227C3ABB1}"/>
+    <hyperlink ref="K25" r:id="rId43" xr:uid="{F9D080CD-142B-443B-ABD0-D6A755886BB2}"/>
+    <hyperlink ref="J26" r:id="rId44" xr:uid="{793B7E3D-F72F-4E0A-93D6-73D47105EEDA}"/>
+    <hyperlink ref="K26" r:id="rId45" xr:uid="{A220C75B-2B93-4FFA-83FF-80385D4BAC5E}"/>
+    <hyperlink ref="J20" r:id="rId46" xr:uid="{A07C5993-29BD-4CE4-8ACD-DDFE88D68FB2}"/>
+    <hyperlink ref="K20" r:id="rId47" xr:uid="{D0A9BC38-F839-4D2F-93B9-A62B36C3CEBF}"/>
+    <hyperlink ref="J27" r:id="rId48" xr:uid="{F9ADDC0D-81CF-4E42-B964-63D4FD61BA13}"/>
+    <hyperlink ref="K27" r:id="rId49" xr:uid="{4F87CAEC-7381-4AAC-92D2-751506D3A161}"/>
+    <hyperlink ref="L15" r:id="rId50" xr:uid="{DECFA331-29DD-4FE7-8BDB-CDE3B2E95E8E}"/>
+    <hyperlink ref="L24" r:id="rId51" xr:uid="{396BB15D-A498-4E98-A64A-2FE1D5019461}"/>
+    <hyperlink ref="J28" r:id="rId52" xr:uid="{FB34B9B4-55E1-47A1-8E21-A821A00D1EC0}"/>
+    <hyperlink ref="K28" r:id="rId53" xr:uid="{C1060359-9B35-48F1-A2D8-AA3BD374A571}"/>
+    <hyperlink ref="J29" r:id="rId54" xr:uid="{BFE70BF4-2F9A-4802-8E95-A3A3490948A8}"/>
+    <hyperlink ref="K29" r:id="rId55" xr:uid="{CE60DCE8-B339-40F0-B2EF-BD73D4938106}"/>
+    <hyperlink ref="J30" r:id="rId56" xr:uid="{3585C032-D124-4147-B5B7-3F2EF6C6A5DE}"/>
+    <hyperlink ref="K30" r:id="rId57" xr:uid="{F22462B9-9A26-48B6-A0DD-B57066B22C40}"/>
+    <hyperlink ref="J31" r:id="rId58" xr:uid="{187F5B61-0870-420A-BB74-16CAAFC01941}"/>
+    <hyperlink ref="J32" r:id="rId59" xr:uid="{680E5967-C777-4D8D-B069-D0D96FFC678B}"/>
+    <hyperlink ref="J33" r:id="rId60" xr:uid="{577FFBCD-009F-478E-8E33-91E761042C29}"/>
+    <hyperlink ref="J34" r:id="rId61" xr:uid="{19F11160-B47A-43B1-9F79-BEA1F1972CA2}"/>
+    <hyperlink ref="K34" r:id="rId62" xr:uid="{752EBF32-C084-4C5C-B069-3517A1A6AE50}"/>
+    <hyperlink ref="J35" r:id="rId63" xr:uid="{9C3C1D94-3708-4CC6-90CF-7C720C888ED2}"/>
+    <hyperlink ref="J36" r:id="rId64" xr:uid="{CDB6AD6E-50EC-4A3E-8C8C-94992C4158F3}"/>
+    <hyperlink ref="J10" r:id="rId65" xr:uid="{93053BC9-17F8-436E-9213-F51AB9B6E7B9}"/>
+    <hyperlink ref="K10" r:id="rId66" xr:uid="{9F468E82-C5AE-4E39-9F04-D83D9BBA1B10}"/>
+    <hyperlink ref="J37" r:id="rId67" xr:uid="{4E2A20E9-461E-4284-A5AB-7343EFE0B405}"/>
+    <hyperlink ref="K37" r:id="rId68" xr:uid="{67FA0A22-1031-4969-A090-A548A959F36B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId67"/>
+  <pageSetup orientation="portrait" r:id="rId69"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Layed out tracker board
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github.com\zachdeibert\radio-tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D24EDAB-B67A-4711-AA28-9A32DF93915E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9116ACDE-B71D-4206-BC2A-D47D7FAE7252}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B5C8F384-52A8-4954-BEC8-251D2703848F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B5C8F384-52A8-4954-BEC8-251D2703848F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="155">
   <si>
     <t>Part</t>
   </si>
@@ -258,15 +258,6 @@
     <t>30 MHz Crystal</t>
   </si>
   <si>
-    <t>XRCGB30M000F3M00R0</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/murata-electronics/XRCGB30M000F3M00R0/490-5583-1-ND/2368397</t>
-  </si>
-  <si>
-    <t>https://www.murata.com/~/media/webrenewal/campaign/ads/america/timing/p79e.ashx?la=en-us</t>
-  </si>
-  <si>
     <t>ISP Header</t>
   </si>
   <si>
@@ -481,6 +472,30 @@
   </si>
   <si>
     <t>https://belfuse.com/resources/datasheets/circuitprotection/ds-cp-0zcm-series.pdf</t>
+  </si>
+  <si>
+    <t>140mA PTC</t>
+  </si>
+  <si>
+    <t>0ZCG0014FF2C</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/bel-fuse-inc/0ZCG0014FF2C/507-1755-1-ND/4156193</t>
+  </si>
+  <si>
+    <t>https://www.belfuse.com/resources/datasheets/circuitprotection/ds-cp-0zcg-series.pdf</t>
+  </si>
+  <si>
+    <t>50mA PTC</t>
+  </si>
+  <si>
+    <t>0ZCM0005FF2G</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/bel-fuse-inc/0ZCM0005FF2G/507-1816-1-ND/4156260</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/raltron-electronics/RH100-30-000-10-F-1010-TR/2151-RH100-30-000-10-F-1010-TRCT-ND/10272841</t>
   </si>
 </sst>
 </file>
@@ -871,10 +886,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF14E9F-6EA3-4C47-9EC5-A7065BD25A1E}">
-  <dimension ref="A1:L38"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,7 +1208,7 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C10" s="3">
         <v>0.61</v>
@@ -1217,10 +1232,10 @@
         <v>0.61</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1228,7 +1243,7 @@
         <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C11" s="3">
         <v>0.38</v>
@@ -1249,10 +1264,10 @@
         <v>0.38</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1383,7 +1398,7 @@
         <v>57</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1516,10 +1531,10 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B20" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C20" s="3">
         <v>0.33</v>
@@ -1543,10 +1558,10 @@
         <v>0.33</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1554,17 +1569,17 @@
         <v>74</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>140</v>
       </c>
       <c r="C21" s="3">
-        <v>0.35</v>
+        <v>0.42</v>
       </c>
       <c r="D21" s="6">
         <v>1</v>
       </c>
       <c r="G21" s="3">
         <f t="shared" si="1"/>
-        <v>0.35</v>
+        <v>0.42</v>
       </c>
       <c r="H21" s="3">
         <f t="shared" si="0"/>
@@ -1575,18 +1590,18 @@
         <v>0</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>76</v>
+        <v>154</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>77</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C22" s="3">
         <v>0.77</v>
@@ -1607,18 +1622,18 @@
         <v>0</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C23" s="3">
         <v>0.56999999999999995</v>
@@ -1639,18 +1654,18 @@
         <v>0</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B24" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D24" s="6">
         <v>1</v>
@@ -1668,18 +1683,18 @@
         <v>0</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B25" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C25" s="3">
         <v>1.7</v>
@@ -1688,30 +1703,30 @@
         <v>1</v>
       </c>
       <c r="G25" s="3">
-        <f t="shared" ref="G25:G38" si="5">$C25*D25</f>
+        <f t="shared" ref="G25:G40" si="5">$C25*D25</f>
         <v>1.7</v>
       </c>
       <c r="H25" s="3">
-        <f t="shared" ref="H25:H38" si="6">$C25*E25</f>
+        <f t="shared" ref="H25:H40" si="6">$C25*E25</f>
         <v>0</v>
       </c>
       <c r="I25" s="3">
-        <f t="shared" ref="I25:I38" si="7">$C25*F25</f>
+        <f t="shared" ref="I25:I40" si="7">$C25*F25</f>
         <v>0</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C26" s="3">
         <v>0.18</v>
@@ -1732,18 +1747,18 @@
         <v>0</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" t="s">
         <v>100</v>
-      </c>
-      <c r="B27" t="s">
-        <v>103</v>
       </c>
       <c r="C27" s="3">
         <v>0.26</v>
@@ -1764,18 +1779,18 @@
         <v>0</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B28" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C28" s="3">
         <v>0.48</v>
@@ -1796,18 +1811,18 @@
         <v>0</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B29" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C29" s="3">
         <v>0.76</v>
@@ -1828,18 +1843,18 @@
         <v>0</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B30" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C30" s="3">
         <v>0.28000000000000003</v>
@@ -1860,18 +1875,18 @@
         <v>0</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B31" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C31" s="3">
         <v>3.48</v>
@@ -1892,15 +1907,15 @@
         <v>0</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>116</v>
+      </c>
+      <c r="B32" t="s">
         <v>119</v>
-      </c>
-      <c r="B32" t="s">
-        <v>122</v>
       </c>
       <c r="C32" s="3">
         <v>0.124</v>
@@ -1921,15 +1936,15 @@
         <v>0</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B33" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C33" s="3">
         <v>0.78</v>
@@ -1950,15 +1965,15 @@
         <v>0</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B34" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C34" s="3">
         <v>0.14000000000000001</v>
@@ -1979,18 +1994,18 @@
         <v>0</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B35" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C35" s="3">
         <v>0.22</v>
@@ -2011,15 +2026,15 @@
         <v>0</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>128</v>
+      </c>
+      <c r="B36" t="s">
         <v>131</v>
-      </c>
-      <c r="B36" t="s">
-        <v>134</v>
       </c>
       <c r="C36" s="3">
         <v>0.45</v>
@@ -2040,15 +2055,15 @@
         <v>0</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B37" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C37" s="3">
         <v>0.7</v>
@@ -2069,28 +2084,31 @@
         <v>0</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B38" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C38" s="3">
         <v>0.16</v>
       </c>
+      <c r="D38" s="6">
+        <v>1</v>
+      </c>
       <c r="F38" s="6">
         <v>1</v>
       </c>
       <c r="G38" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="H38" s="3">
         <f t="shared" si="6"/>
@@ -2101,10 +2119,74 @@
         <v>0.16</v>
       </c>
       <c r="J38" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>147</v>
+      </c>
+      <c r="B39" t="s">
         <v>148</v>
       </c>
-      <c r="K38" s="2" t="s">
+      <c r="C39" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D39" s="6">
+        <v>1</v>
+      </c>
+      <c r="G39" s="3">
+        <f t="shared" si="5"/>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H39" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I39" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J39" s="2" t="s">
         <v>149</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>151</v>
+      </c>
+      <c r="B40" t="s">
+        <v>152</v>
+      </c>
+      <c r="C40" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="D40" s="6">
+        <v>5</v>
+      </c>
+      <c r="G40" s="3">
+        <f t="shared" si="5"/>
+        <v>0.8</v>
+      </c>
+      <c r="H40" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I40" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2144,46 +2226,50 @@
     <hyperlink ref="K18" r:id="rId30" xr:uid="{A24890BF-4B5E-40CB-B9B4-34A68264736E}"/>
     <hyperlink ref="J19" r:id="rId31" xr:uid="{8FB6D7D0-23A7-4B02-9810-79304E9FC6DF}"/>
     <hyperlink ref="K19" r:id="rId32" xr:uid="{F3CA4998-91B4-4D7B-B5CE-EAA22B63412F}"/>
-    <hyperlink ref="J21" r:id="rId33" xr:uid="{7FB55ABB-ED42-4074-86E4-CB5588011F6F}"/>
-    <hyperlink ref="K21" r:id="rId34" xr:uid="{41D3F80A-03BC-477F-82CF-CEBE0D8D65D8}"/>
-    <hyperlink ref="J22" r:id="rId35" xr:uid="{BCD256D2-392F-4BA1-98E8-DAF9918681E6}"/>
-    <hyperlink ref="K22" r:id="rId36" xr:uid="{EED098FB-1018-4864-93D7-093FBEA1E075}"/>
-    <hyperlink ref="J23" r:id="rId37" xr:uid="{866D5E06-28C5-4774-B325-4596BE7F026E}"/>
-    <hyperlink ref="K23" r:id="rId38" xr:uid="{F1429A52-5972-4235-BA2E-8ABDEDFB6995}"/>
-    <hyperlink ref="K24" r:id="rId39" xr:uid="{62B17503-CC61-45E9-91BF-3B440A5FF457}"/>
-    <hyperlink ref="J25" r:id="rId40" xr:uid="{754A96EE-B03B-46E4-A496-9A8227C3ABB1}"/>
-    <hyperlink ref="K25" r:id="rId41" xr:uid="{F9D080CD-142B-443B-ABD0-D6A755886BB2}"/>
-    <hyperlink ref="J26" r:id="rId42" xr:uid="{793B7E3D-F72F-4E0A-93D6-73D47105EEDA}"/>
-    <hyperlink ref="K26" r:id="rId43" xr:uid="{A220C75B-2B93-4FFA-83FF-80385D4BAC5E}"/>
-    <hyperlink ref="J20" r:id="rId44" xr:uid="{A07C5993-29BD-4CE4-8ACD-DDFE88D68FB2}"/>
-    <hyperlink ref="K20" r:id="rId45" xr:uid="{D0A9BC38-F839-4D2F-93B9-A62B36C3CEBF}"/>
-    <hyperlink ref="J27" r:id="rId46" xr:uid="{F9ADDC0D-81CF-4E42-B964-63D4FD61BA13}"/>
-    <hyperlink ref="K27" r:id="rId47" xr:uid="{4F87CAEC-7381-4AAC-92D2-751506D3A161}"/>
-    <hyperlink ref="L15" r:id="rId48" xr:uid="{DECFA331-29DD-4FE7-8BDB-CDE3B2E95E8E}"/>
-    <hyperlink ref="L24" r:id="rId49" xr:uid="{396BB15D-A498-4E98-A64A-2FE1D5019461}"/>
-    <hyperlink ref="J28" r:id="rId50" xr:uid="{FB34B9B4-55E1-47A1-8E21-A821A00D1EC0}"/>
-    <hyperlink ref="K28" r:id="rId51" xr:uid="{C1060359-9B35-48F1-A2D8-AA3BD374A571}"/>
-    <hyperlink ref="J29" r:id="rId52" xr:uid="{BFE70BF4-2F9A-4802-8E95-A3A3490948A8}"/>
-    <hyperlink ref="K29" r:id="rId53" xr:uid="{CE60DCE8-B339-40F0-B2EF-BD73D4938106}"/>
-    <hyperlink ref="J30" r:id="rId54" xr:uid="{3585C032-D124-4147-B5B7-3F2EF6C6A5DE}"/>
-    <hyperlink ref="K30" r:id="rId55" xr:uid="{F22462B9-9A26-48B6-A0DD-B57066B22C40}"/>
-    <hyperlink ref="J31" r:id="rId56" xr:uid="{187F5B61-0870-420A-BB74-16CAAFC01941}"/>
-    <hyperlink ref="J32" r:id="rId57" xr:uid="{680E5967-C777-4D8D-B069-D0D96FFC678B}"/>
-    <hyperlink ref="J33" r:id="rId58" xr:uid="{577FFBCD-009F-478E-8E33-91E761042C29}"/>
-    <hyperlink ref="J34" r:id="rId59" xr:uid="{19F11160-B47A-43B1-9F79-BEA1F1972CA2}"/>
-    <hyperlink ref="K34" r:id="rId60" xr:uid="{752EBF32-C084-4C5C-B069-3517A1A6AE50}"/>
-    <hyperlink ref="J35" r:id="rId61" xr:uid="{9C3C1D94-3708-4CC6-90CF-7C720C888ED2}"/>
-    <hyperlink ref="J36" r:id="rId62" xr:uid="{CDB6AD6E-50EC-4A3E-8C8C-94992C4158F3}"/>
-    <hyperlink ref="J10" r:id="rId63" xr:uid="{93053BC9-17F8-436E-9213-F51AB9B6E7B9}"/>
-    <hyperlink ref="K10" r:id="rId64" xr:uid="{9F468E82-C5AE-4E39-9F04-D83D9BBA1B10}"/>
-    <hyperlink ref="J37" r:id="rId65" xr:uid="{4E2A20E9-461E-4284-A5AB-7343EFE0B405}"/>
-    <hyperlink ref="K37" r:id="rId66" xr:uid="{67FA0A22-1031-4969-A090-A548A959F36B}"/>
-    <hyperlink ref="J11" r:id="rId67" xr:uid="{B816F5E2-BA1C-4421-AC76-DF0502A34AFB}"/>
-    <hyperlink ref="K11" r:id="rId68" xr:uid="{5CD592A3-CEE0-43DB-8484-F7BA8852596F}"/>
-    <hyperlink ref="J38" r:id="rId69" xr:uid="{34FE781E-CDCA-480E-89B0-34F8112534CD}"/>
-    <hyperlink ref="K38" r:id="rId70" xr:uid="{E5F572C2-35FC-4239-A6F9-AC1C44AC3F01}"/>
+    <hyperlink ref="J22" r:id="rId33" xr:uid="{BCD256D2-392F-4BA1-98E8-DAF9918681E6}"/>
+    <hyperlink ref="K22" r:id="rId34" xr:uid="{EED098FB-1018-4864-93D7-093FBEA1E075}"/>
+    <hyperlink ref="J23" r:id="rId35" xr:uid="{866D5E06-28C5-4774-B325-4596BE7F026E}"/>
+    <hyperlink ref="K23" r:id="rId36" xr:uid="{F1429A52-5972-4235-BA2E-8ABDEDFB6995}"/>
+    <hyperlink ref="K24" r:id="rId37" xr:uid="{62B17503-CC61-45E9-91BF-3B440A5FF457}"/>
+    <hyperlink ref="J25" r:id="rId38" xr:uid="{754A96EE-B03B-46E4-A496-9A8227C3ABB1}"/>
+    <hyperlink ref="K25" r:id="rId39" xr:uid="{F9D080CD-142B-443B-ABD0-D6A755886BB2}"/>
+    <hyperlink ref="J26" r:id="rId40" xr:uid="{793B7E3D-F72F-4E0A-93D6-73D47105EEDA}"/>
+    <hyperlink ref="K26" r:id="rId41" xr:uid="{A220C75B-2B93-4FFA-83FF-80385D4BAC5E}"/>
+    <hyperlink ref="J20" r:id="rId42" xr:uid="{A07C5993-29BD-4CE4-8ACD-DDFE88D68FB2}"/>
+    <hyperlink ref="K20" r:id="rId43" xr:uid="{D0A9BC38-F839-4D2F-93B9-A62B36C3CEBF}"/>
+    <hyperlink ref="J27" r:id="rId44" xr:uid="{F9ADDC0D-81CF-4E42-B964-63D4FD61BA13}"/>
+    <hyperlink ref="K27" r:id="rId45" xr:uid="{4F87CAEC-7381-4AAC-92D2-751506D3A161}"/>
+    <hyperlink ref="L15" r:id="rId46" xr:uid="{DECFA331-29DD-4FE7-8BDB-CDE3B2E95E8E}"/>
+    <hyperlink ref="L24" r:id="rId47" xr:uid="{396BB15D-A498-4E98-A64A-2FE1D5019461}"/>
+    <hyperlink ref="J28" r:id="rId48" xr:uid="{FB34B9B4-55E1-47A1-8E21-A821A00D1EC0}"/>
+    <hyperlink ref="K28" r:id="rId49" xr:uid="{C1060359-9B35-48F1-A2D8-AA3BD374A571}"/>
+    <hyperlink ref="J29" r:id="rId50" xr:uid="{BFE70BF4-2F9A-4802-8E95-A3A3490948A8}"/>
+    <hyperlink ref="K29" r:id="rId51" xr:uid="{CE60DCE8-B339-40F0-B2EF-BD73D4938106}"/>
+    <hyperlink ref="J30" r:id="rId52" xr:uid="{3585C032-D124-4147-B5B7-3F2EF6C6A5DE}"/>
+    <hyperlink ref="K30" r:id="rId53" xr:uid="{F22462B9-9A26-48B6-A0DD-B57066B22C40}"/>
+    <hyperlink ref="J31" r:id="rId54" xr:uid="{187F5B61-0870-420A-BB74-16CAAFC01941}"/>
+    <hyperlink ref="J32" r:id="rId55" xr:uid="{680E5967-C777-4D8D-B069-D0D96FFC678B}"/>
+    <hyperlink ref="J33" r:id="rId56" xr:uid="{577FFBCD-009F-478E-8E33-91E761042C29}"/>
+    <hyperlink ref="J34" r:id="rId57" xr:uid="{19F11160-B47A-43B1-9F79-BEA1F1972CA2}"/>
+    <hyperlink ref="K34" r:id="rId58" xr:uid="{752EBF32-C084-4C5C-B069-3517A1A6AE50}"/>
+    <hyperlink ref="J35" r:id="rId59" xr:uid="{9C3C1D94-3708-4CC6-90CF-7C720C888ED2}"/>
+    <hyperlink ref="J36" r:id="rId60" xr:uid="{CDB6AD6E-50EC-4A3E-8C8C-94992C4158F3}"/>
+    <hyperlink ref="J10" r:id="rId61" xr:uid="{93053BC9-17F8-436E-9213-F51AB9B6E7B9}"/>
+    <hyperlink ref="K10" r:id="rId62" xr:uid="{9F468E82-C5AE-4E39-9F04-D83D9BBA1B10}"/>
+    <hyperlink ref="J37" r:id="rId63" xr:uid="{4E2A20E9-461E-4284-A5AB-7343EFE0B405}"/>
+    <hyperlink ref="K37" r:id="rId64" xr:uid="{67FA0A22-1031-4969-A090-A548A959F36B}"/>
+    <hyperlink ref="J11" r:id="rId65" xr:uid="{B816F5E2-BA1C-4421-AC76-DF0502A34AFB}"/>
+    <hyperlink ref="K11" r:id="rId66" xr:uid="{5CD592A3-CEE0-43DB-8484-F7BA8852596F}"/>
+    <hyperlink ref="J38" r:id="rId67" xr:uid="{34FE781E-CDCA-480E-89B0-34F8112534CD}"/>
+    <hyperlink ref="K38" r:id="rId68" xr:uid="{E5F572C2-35FC-4239-A6F9-AC1C44AC3F01}"/>
+    <hyperlink ref="J39" r:id="rId69" xr:uid="{B8253AF3-C4CA-497C-AE01-0F1194C42653}"/>
+    <hyperlink ref="K39" r:id="rId70" xr:uid="{095C8AB8-50F5-4F90-8D30-EB9760E3A358}"/>
+    <hyperlink ref="J40" r:id="rId71" xr:uid="{1A4209F4-A434-41D7-AA6B-E3F085DD17BC}"/>
+    <hyperlink ref="K40" r:id="rId72" xr:uid="{A7FE40C8-7144-4F1B-98B6-1E39325C2533}"/>
+    <hyperlink ref="J21" r:id="rId73" xr:uid="{99C0BE91-D4BC-48D0-AF81-E8D153FC729A}"/>
+    <hyperlink ref="K21" r:id="rId74" xr:uid="{9BDEAC8E-96CD-4612-A8E6-7E84210D21B7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId71"/>
+  <pageSetup orientation="portrait" r:id="rId75"/>
 </worksheet>
 </file>
</xml_diff>